<commit_message>
Add functionality in JOR
</commit_message>
<xml_diff>
--- a/uploads/format/JORequestForm.xlsx
+++ b/uploads/format/JORequestForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -186,9 +186,6 @@
     <t>WHP</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
     <t>JOB ORDER REQUEST</t>
   </si>
   <si>
@@ -217,14 +214,18 @@
   </si>
   <si>
     <t>Scope of Work</t>
+  </si>
+  <si>
+    <t>Notes:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -418,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -435,76 +436,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +557,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -846,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="C11" sqref="C11:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,30 +887,30 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -909,14 +918,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -924,136 +933,132 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="29"/>
+      <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
-      <c r="H7" s="9" t="s">
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="H8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="39"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="H8" s="9" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="I9" s="32"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="H9" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="29"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="33"/>
+      <c r="B13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1061,119 +1066,135 @@
         <v>6</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="J13" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K13" s="33"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="27"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="29"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="29"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I9:K9"/>
+  <mergeCells count="37">
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="C2:H2"/>
@@ -1184,6 +1205,19 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="I7:K7"/>
     <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
excel file update format JOR
</commit_message>
<xml_diff>
--- a/uploads/format/JORequestForm.xlsx
+++ b/uploads/format/JORequestForm.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephine\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\purchasing\uploads\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Central Negros Power Reliability, Inc.</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Requested By:</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Refer to department code sheet</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,10 +448,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,70 +463,70 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -563,7 +572,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E2470C10-039B-48A4-8559-E52AA07AE7F7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -864,7 +873,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:K21"/>
+      <selection activeCell="C7" sqref="C7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,14 +903,14 @@
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="12"/>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="5"/>
@@ -909,14 +918,14 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="6"/>
@@ -924,14 +933,14 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="6"/>
@@ -939,134 +948,142 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
       <c r="H7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="20"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="25"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="26"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
+      <c r="C8" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
       <c r="H8" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="25"/>
+      <c r="I8" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="26"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="41"/>
       <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="25"/>
+      <c r="I9" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="37"/>
+      <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
       <c r="H10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="25"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="25"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="16"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1076,142 +1093,119 @@
       <c r="I13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="33"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="25"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="13"/>
       <c r="H16" s="14"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="25"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="17"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="25"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="25"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="17"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="25"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="17"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="25"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="25"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="17"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="25"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="25"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="I9:K9"/>
@@ -1227,6 +1221,29 @@
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:K11"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>